<commit_message>
more updates to the plots
working on log log plots
</commit_message>
<xml_diff>
--- a/testResults.xlsx
+++ b/testResults.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="8">
   <si>
     <t>N</t>
   </si>
@@ -32,6 +32,12 @@
   </si>
   <si>
     <t>Linear</t>
+  </si>
+  <si>
+    <t>logn</t>
+  </si>
+  <si>
+    <t>logtime</t>
   </si>
 </sst>
 </file>
@@ -84,10 +90,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -342,11 +348,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2101975472"/>
-        <c:axId val="-2101974928"/>
+        <c:axId val="1885303952"/>
+        <c:axId val="1885289264"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2101975472"/>
+        <c:axId val="1885303952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -459,12 +465,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2101974928"/>
+        <c:crossAx val="1885289264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2101974928"/>
+        <c:axId val="1885289264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -577,7 +583,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2101975472"/>
+        <c:crossAx val="1885303952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -863,11 +869,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2103536080"/>
-        <c:axId val="-2103538256"/>
+        <c:axId val="1885293072"/>
+        <c:axId val="1885293616"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2103536080"/>
+        <c:axId val="1885293072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -980,12 +986,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2103538256"/>
+        <c:crossAx val="1885293616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2103538256"/>
+        <c:axId val="1885293616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1098,7 +1104,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2103536080"/>
+        <c:crossAx val="1885293072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1388,11 +1394,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1916052416"/>
-        <c:axId val="-1916049696"/>
+        <c:axId val="1883273616"/>
+        <c:axId val="2046421984"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1916052416"/>
+        <c:axId val="1883273616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1512,12 +1518,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1916049696"/>
+        <c:crossAx val="2046421984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1916049696"/>
+        <c:axId val="2046421984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1630,7 +1636,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1916052416"/>
+        <c:crossAx val="1883273616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1919,11 +1925,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2103536624"/>
-        <c:axId val="-2103537712"/>
+        <c:axId val="2046413280"/>
+        <c:axId val="2046412736"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2103536624"/>
+        <c:axId val="2046413280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2036,12 +2042,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2103537712"/>
+        <c:crossAx val="2046412736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2103537712"/>
+        <c:axId val="2046412736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2129,7 +2135,790 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2103536624"/>
+        <c:crossAx val="2046413280"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Enumerative Log Log Plot</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.5456036745406824E-2"/>
+          <c:y val="0.17634259259259263"/>
+          <c:w val="0.89205796150481187"/>
+          <c:h val="0.77736111111111106"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="8.3370516185476817E-3"/>
+                  <c:y val="-1.9448089822105569E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$N$3:$N$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.3010299956639813</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.6989700043360187</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.3010299956639813</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.4771212547196626</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.6989700043360187</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.0791812460476247</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.1760912590556813</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.3010299956639813</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$O$3:$O$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>-4.0969100130080562</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-3.2311310784251583</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-2.5079066155366894</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-1.7251951799607446</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-1.2764523853917105</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.66682712503302444</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.16469851988853748</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.41441470965579752</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.69515456479056525</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0668237856381992</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1885292528"/>
+        <c:axId val="1885290352"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1885292528"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="t"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1885290352"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1885290352"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1885292528"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Iterative Log Log Plot</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$Q$3:$Q$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.3010299956639813</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.6989700043360187</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.3010299956639813</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.4771212547196626</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.6989700043360187</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.0791812460476247</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.1760912590556813</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.3010299956639813</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$R$3:$R$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>-4.5917600346881509</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-3.8414490005662167</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-3.4708769928917347</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-2.9080392530018351</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-2.6100355017803576</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-2.0888646601947123</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-1.5290206584628074</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-1.3865031258771976</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-1.2059666464164092</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.93486706217082138</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2046418176"/>
+        <c:axId val="2046420896"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2046418176"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2046420896"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2046420896"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2046418176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2338,6 +3127,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -3887,6 +4756,1038 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4524,6 +6425,66 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>166687</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>471487</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="Chart 10"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>14287</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>319087</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="12" name="Chart 11"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4814,10 +6775,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:X12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:H12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4825,316 +6786,680 @@
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="D1" s="1" t="s">
+      <c r="B1" s="2"/>
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="G1" s="1" t="s">
+      <c r="E1" s="2"/>
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1"/>
-      <c r="J1" s="1" t="s">
+      <c r="H1" s="2"/>
+      <c r="J1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="1"/>
+      <c r="K1" s="2"/>
+      <c r="N1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" s="2"/>
+      <c r="Q1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="R1" s="2"/>
+      <c r="T1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U1" s="2"/>
+      <c r="W1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="X1" s="2"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="N2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>20</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>8.0000000000000007E-5</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>20</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <v>2.5599999999999999E-5</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="1">
         <v>20</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="1">
         <v>6.0000000000000002E-5</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3" s="1">
         <v>20</v>
       </c>
-      <c r="K3" s="2">
+      <c r="K3" s="1">
         <v>3.0000000000000001E-6</v>
       </c>
+      <c r="N3" s="1">
+        <f>LOG(A3)</f>
+        <v>1.3010299956639813</v>
+      </c>
+      <c r="O3" s="1">
+        <f>LOG(B3)</f>
+        <v>-4.0969100130080562</v>
+      </c>
+      <c r="Q3" s="1">
+        <f>LOG(D3)</f>
+        <v>1.3010299956639813</v>
+      </c>
+      <c r="R3" s="1">
+        <f>LOG(E3)</f>
+        <v>-4.5917600346881509</v>
+      </c>
+      <c r="T3" s="1">
+        <f>LOG(G3)</f>
+        <v>1.3010299956639813</v>
+      </c>
+      <c r="U3" s="1">
+        <f>LOG(H3)</f>
+        <v>-4.2218487496163561</v>
+      </c>
+      <c r="W3" s="1">
+        <f>LOG(J3)</f>
+        <v>1.3010299956639813</v>
+      </c>
+      <c r="X3" s="1">
+        <f>LOG(K3)</f>
+        <v>-5.5228787452803374</v>
+      </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>50</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>5.8731206370300001E-4</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>50</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="1">
         <v>1.4406251737000001E-4</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="1">
         <v>50</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="1">
         <v>1.6935114846899999E-4</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="1">
         <v>50</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4" s="1">
         <v>5.0000000000000004E-6</v>
       </c>
+      <c r="N4" s="1">
+        <f t="shared" ref="N4:N12" si="0">LOG(A4)</f>
+        <v>1.6989700043360187</v>
+      </c>
+      <c r="O4" s="1">
+        <f t="shared" ref="O4:O12" si="1">LOG(B4)</f>
+        <v>-3.2311310784251583</v>
+      </c>
+      <c r="Q4" s="1">
+        <f t="shared" ref="Q4:Q12" si="2">LOG(D4)</f>
+        <v>1.6989700043360187</v>
+      </c>
+      <c r="R4" s="1">
+        <f t="shared" ref="R4:R12" si="3">LOG(E4)</f>
+        <v>-3.8414490005662167</v>
+      </c>
+      <c r="T4" s="1">
+        <f t="shared" ref="T4:T12" si="4">LOG(G4)</f>
+        <v>1.6989700043360187</v>
+      </c>
+      <c r="U4" s="1">
+        <f t="shared" ref="U4:U12" si="5">LOG(H4)</f>
+        <v>-3.7712118538049539</v>
+      </c>
+      <c r="W4" s="1">
+        <f t="shared" ref="W4:W12" si="6">LOG(J4)</f>
+        <v>1.6989700043360187</v>
+      </c>
+      <c r="X4" s="1">
+        <f t="shared" ref="X4:X12" si="7">LOG(K4)</f>
+        <v>-5.3010299956639813</v>
+      </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>100</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>3.1052272199200001E-3</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>100</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="1">
         <v>3.3816060133599998E-4</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="1">
         <v>100</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="1">
         <v>4.8678476580599997E-4</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="1">
         <v>100</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5" s="1">
         <v>1.0000000000000001E-5</v>
       </c>
+      <c r="N5" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="O5" s="1">
+        <f t="shared" si="1"/>
+        <v>-2.5079066155366894</v>
+      </c>
+      <c r="Q5" s="1">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="R5" s="1">
+        <f t="shared" si="3"/>
+        <v>-3.4708769928917347</v>
+      </c>
+      <c r="T5" s="1">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="U5" s="1">
+        <f t="shared" si="5"/>
+        <v>-3.3126630217113173</v>
+      </c>
+      <c r="W5" s="1">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="X5" s="1">
+        <f t="shared" si="7"/>
+        <v>-5</v>
+      </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>200</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>1.882802733E-2</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>200</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="1">
         <v>1.23583572939E-3</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="1">
         <v>200</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="1">
         <v>1.54300564076E-3</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6" s="1">
         <v>200</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K6" s="1">
         <v>1.0000000000000001E-5</v>
       </c>
+      <c r="N6" s="1">
+        <f t="shared" si="0"/>
+        <v>2.3010299956639813</v>
+      </c>
+      <c r="O6" s="1">
+        <f t="shared" si="1"/>
+        <v>-1.7251951799607446</v>
+      </c>
+      <c r="Q6" s="1">
+        <f t="shared" si="2"/>
+        <v>2.3010299956639813</v>
+      </c>
+      <c r="R6" s="1">
+        <f t="shared" si="3"/>
+        <v>-2.9080392530018351</v>
+      </c>
+      <c r="T6" s="1">
+        <f t="shared" si="4"/>
+        <v>2.3010299956639813</v>
+      </c>
+      <c r="U6" s="1">
+        <f t="shared" si="5"/>
+        <v>-2.8116324862852227</v>
+      </c>
+      <c r="W6" s="1">
+        <f t="shared" si="6"/>
+        <v>2.3010299956639813</v>
+      </c>
+      <c r="X6" s="1">
+        <f t="shared" si="7"/>
+        <v>-5</v>
+      </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>300</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>5.2911200411699999E-2</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <v>300</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="1">
         <v>2.4545082615699998E-3</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="1">
         <v>300</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="1">
         <v>3.0788551976300002E-3</v>
       </c>
-      <c r="J7" s="2">
+      <c r="J7" s="1">
         <v>300</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K7" s="1">
         <v>2.0000000000000002E-5</v>
       </c>
+      <c r="N7" s="1">
+        <f t="shared" si="0"/>
+        <v>2.4771212547196626</v>
+      </c>
+      <c r="O7" s="1">
+        <f t="shared" si="1"/>
+        <v>-1.2764523853917105</v>
+      </c>
+      <c r="Q7" s="1">
+        <f t="shared" si="2"/>
+        <v>2.4771212547196626</v>
+      </c>
+      <c r="R7" s="1">
+        <f t="shared" si="3"/>
+        <v>-2.6100355017803576</v>
+      </c>
+      <c r="T7" s="1">
+        <f t="shared" si="4"/>
+        <v>2.4771212547196626</v>
+      </c>
+      <c r="U7" s="1">
+        <f t="shared" si="5"/>
+        <v>-2.5116107360234201</v>
+      </c>
+      <c r="W7" s="1">
+        <f t="shared" si="6"/>
+        <v>2.4771212547196626</v>
+      </c>
+      <c r="X7" s="1">
+        <f t="shared" si="7"/>
+        <v>-4.6989700043360187</v>
+      </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>500</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>0.215363884014</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="1">
         <v>500</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="1">
         <v>8.1495821103599996E-3</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="1">
         <v>500</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="1">
         <v>7.7691407424899999E-3</v>
       </c>
-      <c r="J8" s="2">
+      <c r="J8" s="1">
         <v>500</v>
       </c>
-      <c r="K8" s="2">
+      <c r="K8" s="1">
         <v>3.0000000000000001E-5</v>
       </c>
+      <c r="N8" s="1">
+        <f t="shared" si="0"/>
+        <v>2.6989700043360187</v>
+      </c>
+      <c r="O8" s="1">
+        <f t="shared" si="1"/>
+        <v>-0.66682712503302444</v>
+      </c>
+      <c r="Q8" s="1">
+        <f t="shared" si="2"/>
+        <v>2.6989700043360187</v>
+      </c>
+      <c r="R8" s="1">
+        <f t="shared" si="3"/>
+        <v>-2.0888646601947123</v>
+      </c>
+      <c r="T8" s="1">
+        <f t="shared" si="4"/>
+        <v>2.6989700043360187</v>
+      </c>
+      <c r="U8" s="1">
+        <f t="shared" si="5"/>
+        <v>-2.109627010984219</v>
+      </c>
+      <c r="W8" s="1">
+        <f t="shared" si="6"/>
+        <v>2.6989700043360187</v>
+      </c>
+      <c r="X8" s="1">
+        <f t="shared" si="7"/>
+        <v>-4.5228787452803374</v>
+      </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
         <v>1000</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>1.4611625072500001</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="1">
         <v>1000</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="1">
         <v>2.9578717635500001E-2</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="1">
         <v>1000</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="1">
         <v>3.05244326095E-2</v>
       </c>
-      <c r="J9" s="2">
+      <c r="J9" s="1">
         <v>1000</v>
       </c>
-      <c r="K9" s="2">
+      <c r="K9" s="1">
         <v>6.9999999999999994E-5</v>
       </c>
+      <c r="N9" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="O9" s="1">
+        <f t="shared" si="1"/>
+        <v>0.16469851988853748</v>
+      </c>
+      <c r="Q9" s="1">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="R9" s="1">
+        <f t="shared" si="3"/>
+        <v>-1.5290206584628074</v>
+      </c>
+      <c r="T9" s="1">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="U9" s="1">
+        <f t="shared" si="5"/>
+        <v>-1.5153524000072702</v>
+      </c>
+      <c r="W9" s="1">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="X9" s="1">
+        <f t="shared" si="7"/>
+        <v>-4.1549019599857431</v>
+      </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
         <v>1200</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>2.5966577381899998</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="1">
         <v>1200</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="1">
         <v>4.1067368399999998E-2</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="1">
         <v>1200</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10" s="1">
         <v>4.3726751636800003E-2</v>
       </c>
-      <c r="J10" s="2">
+      <c r="J10" s="1">
         <v>1200</v>
       </c>
-      <c r="K10" s="2">
+      <c r="K10" s="1">
         <v>8.0000000000000007E-5</v>
       </c>
+      <c r="N10" s="1">
+        <f t="shared" si="0"/>
+        <v>3.0791812460476247</v>
+      </c>
+      <c r="O10" s="1">
+        <f t="shared" si="1"/>
+        <v>0.41441470965579752</v>
+      </c>
+      <c r="Q10" s="1">
+        <f t="shared" si="2"/>
+        <v>3.0791812460476247</v>
+      </c>
+      <c r="R10" s="1">
+        <f t="shared" si="3"/>
+        <v>-1.3865031258771976</v>
+      </c>
+      <c r="T10" s="1">
+        <f t="shared" si="4"/>
+        <v>3.0791812460476247</v>
+      </c>
+      <c r="U10" s="1">
+        <f t="shared" si="5"/>
+        <v>-1.3592527842287145</v>
+      </c>
+      <c r="W10" s="1">
+        <f t="shared" si="6"/>
+        <v>3.0791812460476247</v>
+      </c>
+      <c r="X10" s="1">
+        <f t="shared" si="7"/>
+        <v>-4.0969100130080562</v>
+      </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
         <v>1500</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <v>4.9562655220699998</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="1">
         <v>1500</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="1">
         <v>6.2234807933300003E-2</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11" s="1">
         <v>1500</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11" s="1">
         <v>7.0404860434999994E-2</v>
       </c>
-      <c r="J11" s="2">
+      <c r="J11" s="1">
         <v>1500</v>
       </c>
-      <c r="K11" s="2">
+      <c r="K11" s="1">
         <v>1.1617944950000001E-4</v>
       </c>
+      <c r="N11" s="1">
+        <f t="shared" si="0"/>
+        <v>3.1760912590556813</v>
+      </c>
+      <c r="O11" s="1">
+        <f t="shared" si="1"/>
+        <v>0.69515456479056525</v>
+      </c>
+      <c r="Q11" s="1">
+        <f t="shared" si="2"/>
+        <v>3.1760912590556813</v>
+      </c>
+      <c r="R11" s="1">
+        <f t="shared" si="3"/>
+        <v>-1.2059666464164092</v>
+      </c>
+      <c r="T11" s="1">
+        <f t="shared" si="4"/>
+        <v>3.1760912590556813</v>
+      </c>
+      <c r="U11" s="1">
+        <f t="shared" si="5"/>
+        <v>-1.1523973580846445</v>
+      </c>
+      <c r="W11" s="1">
+        <f t="shared" si="6"/>
+        <v>3.1760912590556813</v>
+      </c>
+      <c r="X11" s="1">
+        <f t="shared" si="7"/>
+        <v>-3.9348706856983053</v>
+      </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
         <v>2000</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="1">
         <v>11.663362817699999</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="1">
         <v>2000</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="1">
         <v>0.11618041884499999</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12" s="1">
         <v>2000</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12" s="1">
         <v>0.12733624043299999</v>
       </c>
-      <c r="J12" s="2">
+      <c r="J12" s="1">
         <v>2000</v>
       </c>
-      <c r="K12" s="2">
+      <c r="K12" s="1">
         <v>1.69436679354E-4</v>
+      </c>
+      <c r="N12" s="1">
+        <f t="shared" si="0"/>
+        <v>3.3010299956639813</v>
+      </c>
+      <c r="O12" s="1">
+        <f t="shared" si="1"/>
+        <v>1.0668237856381992</v>
+      </c>
+      <c r="Q12" s="1">
+        <f t="shared" si="2"/>
+        <v>3.3010299956639813</v>
+      </c>
+      <c r="R12" s="1">
+        <f t="shared" si="3"/>
+        <v>-0.93486706217082138</v>
+      </c>
+      <c r="T12" s="1">
+        <f t="shared" si="4"/>
+        <v>3.3010299956639813</v>
+      </c>
+      <c r="U12" s="1">
+        <f t="shared" si="5"/>
+        <v>-0.89504797670639713</v>
+      </c>
+      <c r="W12" s="1">
+        <f t="shared" si="6"/>
+        <v>3.3010299956639813</v>
+      </c>
+      <c r="X12" s="1">
+        <f t="shared" si="7"/>
+        <v>-3.770992568522979</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="8">
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="W1:X1"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="J1:K1"/>
+    <mergeCell ref="N1:O1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
added some more work to experimental analysis
also added a plot of all four algorithms together
</commit_message>
<xml_diff>
--- a/testResults.xlsx
+++ b/testResults.xlsx
@@ -8,14 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
   <si>
     <t>N</t>
   </si>
@@ -34,12 +34,24 @@
   <si>
     <t>Linear</t>
   </si>
+  <si>
+    <t>Enumerative Time</t>
+  </si>
+  <si>
+    <t>Iterative Time</t>
+  </si>
+  <si>
+    <t>Divide/Conquer Time</t>
+  </si>
+  <si>
+    <t>Linear Time</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -54,18 +66,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -75,7 +75,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -98,84 +98,17 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,11 +363,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1988578144"/>
-        <c:axId val="1986557888"/>
+        <c:axId val="475446224"/>
+        <c:axId val="475442416"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1988578144"/>
+        <c:axId val="475446224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -547,12 +480,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1986557888"/>
+        <c:crossAx val="475442416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1986557888"/>
+        <c:axId val="475442416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -665,7 +598,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1988578144"/>
+        <c:crossAx val="475446224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -951,11 +884,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="4286512"/>
-        <c:axId val="4279440"/>
+        <c:axId val="475444592"/>
+        <c:axId val="475445136"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="4286512"/>
+        <c:axId val="475444592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1068,12 +1001,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="4279440"/>
+        <c:crossAx val="475445136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="4279440"/>
+        <c:axId val="475445136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1186,7 +1119,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="4286512"/>
+        <c:crossAx val="475444592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1476,11 +1409,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="4272368"/>
-        <c:axId val="4274000"/>
+        <c:axId val="475456016"/>
+        <c:axId val="475447312"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="4272368"/>
+        <c:axId val="475456016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1600,12 +1533,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="4274000"/>
+        <c:crossAx val="475447312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="4274000"/>
+        <c:axId val="475447312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1718,7 +1651,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="4272368"/>
+        <c:crossAx val="475456016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2007,11 +1940,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="4285968"/>
-        <c:axId val="4274544"/>
+        <c:axId val="475450032"/>
+        <c:axId val="475452208"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="4285968"/>
+        <c:axId val="475450032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2124,12 +2057,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="4274544"/>
+        <c:crossAx val="475452208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="4274544"/>
+        <c:axId val="475452208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2217,7 +2150,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="4285968"/>
+        <c:crossAx val="475450032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2229,6 +2162,1750 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>All Four Algorithms</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Enumerative Time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$B$2:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>8.0000000000000007E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.8731206370300001E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.1052272199200001E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.882802733E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.2911200411699999E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.215363884014</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.4611625072500001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.5966577381899998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.9562655220699998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11.663362817699999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Iterative Time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$C$2:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2.5599999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.4406251737000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.3816060133599998E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.23583572939E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.4545082615699998E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.1495821103599996E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.9578717635500001E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.1067368399999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.2234807933300003E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.11618041884499999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Divide/Conquer Time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$D$2:$D$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>6.0000000000000002E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.6935114846899999E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.8678476580599997E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.54300564076E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.0788551976300002E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.7691407424899999E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.05244326095E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.3726751636800003E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.0404860434999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.12733624043299999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Linear Time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$E$2:$E$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>3.0000000000000001E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0000000000000004E-6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0000000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0000000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0000000000000002E-5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.0000000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.9999999999999994E-5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0000000000000007E-5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.1617944950000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.69436679354E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="661150144"/>
+        <c:axId val="661134368"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="661150144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Size of N</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="661134368"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="661134368"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> in Seconds</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="661150144"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:minorUnit val="1.0000000000000002E-2"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>All Four Algorithms</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Enumerative Time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$B$2:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>8.0000000000000007E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.8731206370300001E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.1052272199200001E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.882802733E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.2911200411699999E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.215363884014</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.4611625072500001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.5966577381899998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.9562655220699998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11.663362817699999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Iterative Time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$C$2:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2.5599999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.4406251737000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.3816060133599998E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.23583572939E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.4545082615699998E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.1495821103599996E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.9578717635500001E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.1067368399999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.2234807933300003E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.11618041884499999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Divide/Conquer Time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$D$2:$D$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>6.0000000000000002E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.6935114846899999E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.8678476580599997E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.54300564076E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.0788551976300002E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.7691407424899999E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.05244326095E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.3726751636800003E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.0404860434999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.12733624043299999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Linear Time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$E$2:$E$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>3.0000000000000001E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0000000000000004E-6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0000000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0000000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0000000000000002E-5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.0000000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.9999999999999994E-5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0000000000000007E-5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.1617944950000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.69436679354E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="319859952"/>
+        <c:axId val="319857776"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="319859952"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Size of N</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="319857776"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="319857776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> in Seconds</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="319859952"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:minorUnit val="1.0000000000000002E-2"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -2426,6 +4103,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -3975,6 +5732,1038 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4832,6 +7621,73 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>299357</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>108857</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>18370</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>185057</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Chart 9"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>357186</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>152399</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5124,8 +7980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I56" sqref="I56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5134,22 +7990,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="D1" s="2" t="s">
+      <c r="B1" s="3"/>
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="G1" s="2" t="s">
+      <c r="E1" s="3"/>
+      <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="2"/>
-      <c r="J1" s="2" t="s">
+      <c r="H1" s="3"/>
+      <c r="J1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="2"/>
+      <c r="K1" s="3"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -5254,7 +8110,7 @@
       <c r="K5" s="1">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="L5" s="8"/>
+      <c r="L5" s="2"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
@@ -5281,7 +8137,7 @@
       <c r="K6" s="1">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="O6" s="8"/>
+      <c r="O6" s="2"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
@@ -5386,7 +8242,7 @@
       <c r="K10" s="1">
         <v>8.0000000000000007E-5</v>
       </c>
-      <c r="O10" s="8"/>
+      <c r="O10" s="2"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
@@ -5454,180 +8310,209 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection sqref="A1:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3">
-        <v>1</v>
-      </c>
-      <c r="B1" s="4">
-        <v>6.0000000000000002E-6</v>
-      </c>
-      <c r="F1">
-        <f>LOG(A1)</f>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G1">
-        <f t="shared" ref="G1:G10" si="0">LOG(B1)</f>
-        <v>-5.2218487496163561</v>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>20</v>
+      </c>
+      <c r="B2" s="1">
+        <v>8.0000000000000007E-5</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2.5599999999999999E-5</v>
+      </c>
+      <c r="D2" s="1">
+        <v>6.0000000000000002E-5</v>
+      </c>
+      <c r="E2" s="1">
+        <v>3.0000000000000001E-6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>50</v>
+      </c>
+      <c r="B3" s="1">
+        <v>5.8731206370300001E-4</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1.4406251737000001E-4</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1.6935114846899999E-4</v>
+      </c>
+      <c r="E3" s="1">
+        <v>5.0000000000000004E-6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>100</v>
       </c>
-      <c r="B2" s="6">
-        <v>8.0699999999999994E-2</v>
-      </c>
-      <c r="F2">
-        <f t="shared" ref="F2:F10" si="1">LOG(A2)</f>
-        <v>2</v>
-      </c>
-      <c r="G2">
-        <f t="shared" si="0"/>
-        <v>-1.0931264652779296</v>
+      <c r="B4" s="1">
+        <v>3.1052272199200001E-3</v>
+      </c>
+      <c r="C4" s="1">
+        <v>3.3816060133599998E-4</v>
+      </c>
+      <c r="D4" s="1">
+        <v>4.8678476580599997E-4</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5">
-        <v>250</v>
-      </c>
-      <c r="B3" s="6">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="F3">
-        <f t="shared" si="1"/>
-        <v>2.3979400086720375</v>
-      </c>
-      <c r="G3">
-        <f t="shared" si="0"/>
-        <v>4.1392685158225077E-2</v>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>200</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1.882802733E-2</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1.23583572939E-3</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1.54300564076E-3</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>300</v>
+      </c>
+      <c r="B6" s="1">
+        <v>5.2911200411699999E-2</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2.4545082615699998E-3</v>
+      </c>
+      <c r="D6" s="1">
+        <v>3.0788551976300002E-3</v>
+      </c>
+      <c r="E6" s="1">
+        <v>2.0000000000000002E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>500</v>
       </c>
-      <c r="B4" s="6">
-        <v>8.65</v>
-      </c>
-      <c r="F4">
-        <f t="shared" si="1"/>
-        <v>2.6989700043360187</v>
-      </c>
-      <c r="G4">
-        <f t="shared" si="0"/>
-        <v>0.93701610746481423</v>
+      <c r="B7" s="1">
+        <v>0.215363884014</v>
+      </c>
+      <c r="C7" s="1">
+        <v>8.1495821103599996E-3</v>
+      </c>
+      <c r="D7" s="1">
+        <v>7.7691407424899999E-3</v>
+      </c>
+      <c r="E7" s="1">
+        <v>3.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5">
-        <v>750</v>
-      </c>
-      <c r="B5" s="6">
-        <v>29.2</v>
-      </c>
-      <c r="F5">
-        <f t="shared" si="1"/>
-        <v>2.8750612633917001</v>
-      </c>
-      <c r="G5">
-        <f t="shared" si="0"/>
-        <v>1.4653828514484182</v>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>1000</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1.4611625072500001</v>
+      </c>
+      <c r="C8" s="1">
+        <v>2.9578717635500001E-2</v>
+      </c>
+      <c r="D8" s="1">
+        <v>3.05244326095E-2</v>
+      </c>
+      <c r="E8" s="1">
+        <v>6.9999999999999994E-5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="5">
-        <v>1000</v>
-      </c>
-      <c r="B6" s="6">
-        <v>62.9</v>
-      </c>
-      <c r="F6">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="G6">
-        <f t="shared" si="0"/>
-        <v>1.7986506454452689</v>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>1200</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2.5966577381899998</v>
+      </c>
+      <c r="C9" s="1">
+        <v>4.1067368399999998E-2</v>
+      </c>
+      <c r="D9" s="1">
+        <v>4.3726751636800003E-2</v>
+      </c>
+      <c r="E9" s="1">
+        <v>8.0000000000000007E-5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="5">
-        <v>1250</v>
-      </c>
-      <c r="B7" s="6">
-        <v>124</v>
-      </c>
-      <c r="F7">
-        <f t="shared" si="1"/>
-        <v>3.0969100130080562</v>
-      </c>
-      <c r="G7">
-        <f t="shared" si="0"/>
-        <v>2.0934216851622351</v>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>1500</v>
+      </c>
+      <c r="B10" s="1">
+        <v>4.9562655220699998</v>
+      </c>
+      <c r="C10" s="1">
+        <v>6.2234807933300003E-2</v>
+      </c>
+      <c r="D10" s="1">
+        <v>7.0404860434999994E-2</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1.1617944950000001E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="5">
-        <v>1500</v>
-      </c>
-      <c r="B8" s="6">
-        <v>218</v>
-      </c>
-      <c r="F8">
-        <f t="shared" si="1"/>
-        <v>3.1760912590556813</v>
-      </c>
-      <c r="G8">
-        <f t="shared" si="0"/>
-        <v>2.3384564936046046</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="5">
-        <v>1750</v>
-      </c>
-      <c r="B9" s="6">
-        <v>380.41</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="1"/>
-        <v>3.2430380486862944</v>
-      </c>
-      <c r="G9">
-        <f t="shared" si="0"/>
-        <v>2.5802519248998035</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
         <v>2000</v>
       </c>
-      <c r="B10" s="7">
-        <v>564.58000000000004</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="1"/>
-        <v>3.3010299956639813</v>
-      </c>
-      <c r="G10">
-        <f t="shared" si="0"/>
-        <v>2.7517254893909873</v>
+      <c r="B11" s="1">
+        <v>11.663362817699999</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0.11618041884499999</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.12733624043299999</v>
+      </c>
+      <c r="E11" s="1">
+        <v>1.69436679354E-4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>